<commit_message>
Fixed the Annual Read-in and added download button
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_annual.xlsx
+++ b/code/paleo_flow/data/sites_annual.xlsx
@@ -81,106 +81,106 @@
     <t>https://waterdata.usgs.gov/nwis/uv?site_no=10011500</t>
   </si>
   <si>
+    <t>Logan River</t>
+  </si>
+  <si>
+    <t>Logan River, Utah 400 Year Streamflow Reconstructions</t>
+  </si>
+  <si>
+    <t>Allen, E.B.; Rittenour, T.M.; DeRose, R.J.; Bekker, M.F.; Kjelgren, R.; Buckley, B.M.</t>
+  </si>
+  <si>
+    <t>Eric B. Allen, Tammy M. Rittenour, R. Justin DeRose, Matthew F. Bekker, Roger Kjelgren, Brendan M. Buckley. 2013. A tree-ring based reconstruction of Logan River streamflow, northern Utah. Water Resources Research, 49(12), 8579-8588. doi: 10.1002/2013WR014273</t>
+  </si>
+  <si>
+    <t>https://www.ncdc.noaa.gov/paleo-search/study/16074</t>
+  </si>
+  <si>
+    <t>USGS 10109001</t>
+  </si>
+  <si>
+    <t>https://waterdata.usgs.gov/nwis/dv?referred_module=sw&amp;site_no=10109001</t>
+  </si>
+  <si>
+    <t>Weber River</t>
+  </si>
+  <si>
+    <t>Weber River, Utah 576 Year Streamflow Reconstruction</t>
+  </si>
+  <si>
+    <t>Bekker, M.F.; DeRose, R.J.; Buckley, B.M.; Kjelgren, R.; Gill, N.S.</t>
+  </si>
+  <si>
+    <t>Matthew F. Bekker, R. Justin DeRose, Brendan M. Buckley, Roger K. Kjelgren, and Nathan S. Gill. 2014. A 576-Year Weber River Streamflow Reconstruction from Tree Rings for Water Resource Risk Assessment in the Wasatch Front, Utah. Journal of the American Water Resources Association. . doi: 10.1111/jawr.12191</t>
+  </si>
+  <si>
+    <t>https://www.ncdc.noaa.gov/paleo-search/study/16416</t>
+  </si>
+  <si>
+    <t>USGS 10128500</t>
+  </si>
+  <si>
+    <t>https://waterdata.usgs.gov/nwis/uv?site_no=10128500</t>
+  </si>
+  <si>
+    <t>Yeruu River</t>
+  </si>
+  <si>
+    <t>CO, USA</t>
+  </si>
+  <si>
+    <t>Upper Rio Grande</t>
+  </si>
+  <si>
+    <t>Rio Grande 500 Year Riverflow and Precipitation Reconstructions</t>
+  </si>
+  <si>
+    <t>Woodhouse, C.A.; Meko, D.M.; Griffin, D.; Castro, C.L.</t>
+  </si>
+  <si>
+    <t>Woodhouse, C.A., D.M. Meko, D. Griffin, and C.L. Castro. 2013. Tree rings and multiseason drought variability in the lower Rio Grande Basin, USA. Water Resources Research, Vol. 49, Issue 2, pp. 844-850. DOI: 10.1002/wrcr.20098</t>
+  </si>
+  <si>
+    <t>https://www.ncdc.noaa.gov/paleo-search/study/14249</t>
+  </si>
+  <si>
+    <t>USGS 08220000</t>
+  </si>
+  <si>
+    <t>flow_08220000</t>
+  </si>
+  <si>
+    <t>https://waterdata.usgs.gov/nwis/inventory/?site_no=08220000</t>
+  </si>
+  <si>
+    <t>flow_yeruu</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>yeruu</t>
+  </si>
+  <si>
+    <t>Yeruu River, Mongolia 300 Year Streamflow Reconstruction</t>
+  </si>
+  <si>
+    <t>Pederson, N.; Leland, C.; Nachin, B.; Hessl, A.E.; Bell, A.R.; Martin-Benito, D.; Saladyga, T.; Suran, B.; Brown, P.M.; Davi, N.K.</t>
+  </si>
+  <si>
+    <t>Pederson, N., C. Leland, B. Nachin, A.E. Hessl, A.R. Bell, D. Martin-Benito, T. Saladyga, B. Suran, P.M. Brown, N.K. Davi. 2012. Three centuries of shifting hydroclimatic regimes across the Mongolian Breadbasket. Agricultural and Forest Meteorology, DOI: 10.1016/j.agrformet.2012.07.003.</t>
+  </si>
+  <si>
+    <t>https://www.ncdc.noaa.gov/paleo-search/study/13542</t>
+  </si>
+  <si>
     <t>flow_10011500</t>
   </si>
   <si>
-    <t>Logan River</t>
-  </si>
-  <si>
-    <t>Logan River, Utah 400 Year Streamflow Reconstructions</t>
-  </si>
-  <si>
-    <t>Allen, E.B.; Rittenour, T.M.; DeRose, R.J.; Bekker, M.F.; Kjelgren, R.; Buckley, B.M.</t>
-  </si>
-  <si>
-    <t>Eric B. Allen, Tammy M. Rittenour, R. Justin DeRose, Matthew F. Bekker, Roger Kjelgren, Brendan M. Buckley. 2013. A tree-ring based reconstruction of Logan River streamflow, northern Utah. Water Resources Research, 49(12), 8579-8588. doi: 10.1002/2013WR014273</t>
-  </si>
-  <si>
-    <t>https://www.ncdc.noaa.gov/paleo-search/study/16074</t>
-  </si>
-  <si>
-    <t>USGS 10109001</t>
-  </si>
-  <si>
-    <t>https://waterdata.usgs.gov/nwis/dv?referred_module=sw&amp;site_no=10109001</t>
-  </si>
-  <si>
     <t>flow_10109001</t>
   </si>
   <si>
-    <t>Weber River</t>
-  </si>
-  <si>
-    <t>Weber River, Utah 576 Year Streamflow Reconstruction</t>
-  </si>
-  <si>
-    <t>Bekker, M.F.; DeRose, R.J.; Buckley, B.M.; Kjelgren, R.; Gill, N.S.</t>
-  </si>
-  <si>
-    <t>Matthew F. Bekker, R. Justin DeRose, Brendan M. Buckley, Roger K. Kjelgren, and Nathan S. Gill. 2014. A 576-Year Weber River Streamflow Reconstruction from Tree Rings for Water Resource Risk Assessment in the Wasatch Front, Utah. Journal of the American Water Resources Association. . doi: 10.1111/jawr.12191</t>
-  </si>
-  <si>
-    <t>https://www.ncdc.noaa.gov/paleo-search/study/16416</t>
-  </si>
-  <si>
-    <t>USGS 10128500</t>
-  </si>
-  <si>
-    <t>https://waterdata.usgs.gov/nwis/uv?site_no=10128500</t>
-  </si>
-  <si>
     <t>flow_10128500</t>
-  </si>
-  <si>
-    <t>Yeruu River</t>
-  </si>
-  <si>
-    <t>CO, USA</t>
-  </si>
-  <si>
-    <t>Upper Rio Grande</t>
-  </si>
-  <si>
-    <t>Rio Grande 500 Year Riverflow and Precipitation Reconstructions</t>
-  </si>
-  <si>
-    <t>Woodhouse, C.A.; Meko, D.M.; Griffin, D.; Castro, C.L.</t>
-  </si>
-  <si>
-    <t>Woodhouse, C.A., D.M. Meko, D. Griffin, and C.L. Castro. 2013. Tree rings and multiseason drought variability in the lower Rio Grande Basin, USA. Water Resources Research, Vol. 49, Issue 2, pp. 844-850. DOI: 10.1002/wrcr.20098</t>
-  </si>
-  <si>
-    <t>https://www.ncdc.noaa.gov/paleo-search/study/14249</t>
-  </si>
-  <si>
-    <t>USGS 08220000</t>
-  </si>
-  <si>
-    <t>flow_08220000</t>
-  </si>
-  <si>
-    <t>https://waterdata.usgs.gov/nwis/inventory/?site_no=08220000</t>
-  </si>
-  <si>
-    <t>flow_yeruu</t>
-  </si>
-  <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
-    <t>yeruu</t>
-  </si>
-  <si>
-    <t>Yeruu River, Mongolia 300 Year Streamflow Reconstruction</t>
-  </si>
-  <si>
-    <t>Pederson, N.; Leland, C.; Nachin, B.; Hessl, A.E.; Bell, A.R.; Martin-Benito, D.; Saladyga, T.; Suran, B.; Brown, P.M.; Davi, N.K.</t>
-  </si>
-  <si>
-    <t>Pederson, N., C. Leland, B. Nachin, A.E. Hessl, A.R. Bell, D. Martin-Benito, T. Saladyga, B. Suran, P.M. Brown, N.K. Davi. 2012. Three centuries of shifting hydroclimatic regimes across the Mongolian Breadbasket. Agricultural and Forest Meteorology, DOI: 10.1016/j.agrformet.2012.07.003.</t>
-  </si>
-  <si>
-    <t>https://www.ncdc.noaa.gov/paleo-search/study/13542</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -570,37 +570,37 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>8220000</v>
       </c>
       <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -646,31 +646,31 @@
         <v>10109001</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -681,57 +681,57 @@
         <v>10128500</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed default to annual, fixed site ordering extra spaces, US first
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_annual.xlsx
+++ b/code/paleo_flow/data/sites_annual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="782">
   <si>
     <t>site_group</t>
   </si>
@@ -2173,30 +2173,6 @@
     <t>https://waterdata.usgs.gov/nwis/inventory/?site_no=06921200&amp;agency_cd=USGS</t>
   </si>
   <si>
-    <t>USA,  WY</t>
-  </si>
-  <si>
-    <t>USA,  MT</t>
-  </si>
-  <si>
-    <t>USA,  ND</t>
-  </si>
-  <si>
-    <t>USA,  SD</t>
-  </si>
-  <si>
-    <t>USA,  NE</t>
-  </si>
-  <si>
-    <t>USA,  CO</t>
-  </si>
-  <si>
-    <t>USA,  KS</t>
-  </si>
-  <si>
-    <t>USA,  MO</t>
-  </si>
-  <si>
     <t>usgs_06278300</t>
   </si>
   <si>
@@ -2369,6 +2345,21 @@
   </si>
   <si>
     <t>arkansascanoncity_update</t>
+  </si>
+  <si>
+    <t>USA, ND</t>
+  </si>
+  <si>
+    <t>USA, SD</t>
+  </si>
+  <si>
+    <t>USA, NE</t>
+  </si>
+  <si>
+    <t>USA, KS</t>
+  </si>
+  <si>
+    <t>USA, MO</t>
   </si>
 </sst>
 </file>
@@ -3216,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E71" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6287,7 +6278,7 @@
         <v>466</v>
       </c>
       <c r="J84" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="K84">
         <v>38.433889000000001</v>
@@ -6470,7 +6461,7 @@
         <v>548</v>
       </c>
       <c r="G90" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="J90" t="s">
         <v>493</v>
@@ -6513,7 +6504,7 @@
         <v>552</v>
       </c>
       <c r="G92" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="J92" t="s">
         <v>495</v>
@@ -6751,7 +6742,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
         <v>554</v>
@@ -6778,7 +6769,7 @@
         <v>664</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="K100">
         <v>44.508019529999999</v>
@@ -6789,7 +6780,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B101" t="s">
         <v>555</v>
@@ -6816,7 +6807,7 @@
         <v>665</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="K101">
         <v>44.20828238</v>
@@ -6827,7 +6818,7 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" t="s">
-        <v>720</v>
+        <v>542</v>
       </c>
       <c r="B102" t="s">
         <v>556</v>
@@ -6854,7 +6845,7 @@
         <v>666</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="K102">
         <v>45.006909700000001</v>
@@ -6865,7 +6856,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B103" t="s">
         <v>557</v>
@@ -6892,7 +6883,7 @@
         <v>667</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="K103">
         <v>43.577739989999998</v>
@@ -6903,7 +6894,7 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B104" t="s">
         <v>558</v>
@@ -6930,7 +6921,7 @@
         <v>668</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="K104">
         <v>44.027742279999998</v>
@@ -6941,7 +6932,7 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B105" t="s">
         <v>559</v>
@@ -6968,7 +6959,7 @@
         <v>669</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="K105">
         <v>47.78723694</v>
@@ -6979,7 +6970,7 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B106" t="s">
         <v>560</v>
@@ -7006,7 +6997,7 @@
         <v>670</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="K106">
         <v>46.274727800000001</v>
@@ -7017,7 +7008,7 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B107" t="s">
         <v>561</v>
@@ -7044,7 +7035,7 @@
         <v>671</v>
       </c>
       <c r="J107" s="5" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="K107">
         <v>47.236125940000001</v>
@@ -7055,7 +7046,7 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B108" t="s">
         <v>562</v>
@@ -7082,7 +7073,7 @@
         <v>672</v>
       </c>
       <c r="J108" s="5" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="K108">
         <v>47.027791579999999</v>
@@ -7093,7 +7084,7 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B109" t="s">
         <v>563</v>
@@ -7120,7 +7111,7 @@
         <v>673</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="K109">
         <v>46.426671159999998</v>
@@ -7131,7 +7122,7 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B110" t="s">
         <v>564</v>
@@ -7158,7 +7149,7 @@
         <v>674</v>
       </c>
       <c r="J110" s="5" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="K110">
         <v>46.15417025</v>
@@ -7169,7 +7160,7 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B111" t="s">
         <v>565</v>
@@ -7196,7 +7187,7 @@
         <v>675</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="K111">
         <v>46.376111109999997</v>
@@ -7207,7 +7198,7 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B112" t="s">
         <v>566</v>
@@ -7234,7 +7225,7 @@
         <v>676</v>
       </c>
       <c r="J112" s="5" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="K112">
         <v>46.257490050000001</v>
@@ -7245,7 +7236,7 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B113" t="s">
         <v>567</v>
@@ -7272,7 +7263,7 @@
         <v>677</v>
       </c>
       <c r="J113" s="5" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="K113">
         <v>45.255817120000003</v>
@@ -7283,7 +7274,7 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B114" t="s">
         <v>568</v>
@@ -7310,7 +7301,7 @@
         <v>678</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="K114">
         <v>43.828045860000003</v>
@@ -7321,7 +7312,7 @@
     </row>
     <row r="115" spans="1:12">
       <c r="A115" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B115" t="s">
         <v>569</v>
@@ -7348,7 +7339,7 @@
         <v>679</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="K115">
         <v>44.013592379999999</v>
@@ -7359,7 +7350,7 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B116" t="s">
         <v>570</v>
@@ -7386,7 +7377,7 @@
         <v>680</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="K116">
         <v>44.326648970000001</v>
@@ -7397,7 +7388,7 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B117" t="s">
         <v>571</v>
@@ -7424,7 +7415,7 @@
         <v>681</v>
       </c>
       <c r="J117" s="5" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="K117">
         <v>43.752494910000003</v>
@@ -7435,7 +7426,7 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B118" t="s">
         <v>572</v>
@@ -7462,7 +7453,7 @@
         <v>682</v>
       </c>
       <c r="J118" s="5" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="K118">
         <v>43.601385489999998</v>
@@ -7473,7 +7464,7 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B119" t="s">
         <v>573</v>
@@ -7500,7 +7491,7 @@
         <v>683</v>
       </c>
       <c r="J119" s="5" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="K119">
         <v>43.748327449999998</v>
@@ -7511,7 +7502,7 @@
     </row>
     <row r="120" spans="1:12">
       <c r="A120" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B120" t="s">
         <v>574</v>
@@ -7538,7 +7529,7 @@
         <v>684</v>
       </c>
       <c r="J120" s="5" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="K120">
         <v>42.943036110000001</v>
@@ -7549,7 +7540,7 @@
     </row>
     <row r="121" spans="1:12">
       <c r="A121" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B121" t="s">
         <v>575</v>
@@ -7576,7 +7567,7 @@
         <v>685</v>
       </c>
       <c r="J121" s="5" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="K121">
         <v>42.810994440000002</v>
@@ -7587,7 +7578,7 @@
     </row>
     <row r="122" spans="1:12">
       <c r="A122" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B122" t="s">
         <v>576</v>
@@ -7614,7 +7605,7 @@
         <v>686</v>
       </c>
       <c r="J122" s="5" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="K122">
         <v>42.753610799999997</v>
@@ -7625,7 +7616,7 @@
     </row>
     <row r="123" spans="1:12">
       <c r="A123" t="s">
-        <v>721</v>
+        <v>777</v>
       </c>
       <c r="B123" t="s">
         <v>577</v>
@@ -7652,7 +7643,7 @@
         <v>687</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="K123">
         <v>45.938861559999999</v>
@@ -7663,7 +7654,7 @@
     </row>
     <row r="124" spans="1:12">
       <c r="A124" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B124" t="s">
         <v>578</v>
@@ -7690,7 +7681,7 @@
         <v>688</v>
       </c>
       <c r="J124" s="5" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="K124">
         <v>43.776400000000002</v>
@@ -7701,7 +7692,7 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B125" t="s">
         <v>579</v>
@@ -7728,7 +7719,7 @@
         <v>689</v>
       </c>
       <c r="J125" s="5" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="K125">
         <v>43.794144369999998</v>
@@ -7739,7 +7730,7 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" t="s">
-        <v>722</v>
+        <v>778</v>
       </c>
       <c r="B126" t="s">
         <v>580</v>
@@ -7766,7 +7757,7 @@
         <v>690</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="K126">
         <v>45.006075299999999</v>
@@ -7777,7 +7768,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B127" t="s">
         <v>581</v>
@@ -7804,7 +7795,7 @@
         <v>691</v>
       </c>
       <c r="J127" s="5" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="K127">
         <v>42.321580560000001</v>
@@ -7815,7 +7806,7 @@
     </row>
     <row r="128" spans="1:12">
       <c r="A128" t="s">
-        <v>724</v>
+        <v>43</v>
       </c>
       <c r="B128" t="s">
         <v>582</v>
@@ -7842,7 +7833,7 @@
         <v>692</v>
       </c>
       <c r="J128" s="5" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="K128">
         <v>40.49609409</v>
@@ -7853,7 +7844,7 @@
     </row>
     <row r="129" spans="1:12">
       <c r="A129" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B129" t="s">
         <v>583</v>
@@ -7880,7 +7871,7 @@
         <v>693</v>
       </c>
       <c r="J129" s="5" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="K129">
         <v>41.370244710000001</v>
@@ -7891,7 +7882,7 @@
     </row>
     <row r="130" spans="1:12">
       <c r="A130" t="s">
-        <v>719</v>
+        <v>49</v>
       </c>
       <c r="B130" t="s">
         <v>584</v>
@@ -7918,7 +7909,7 @@
         <v>694</v>
       </c>
       <c r="J130" s="5" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="K130">
         <v>41.585245489999998</v>
@@ -7929,7 +7920,7 @@
     </row>
     <row r="131" spans="1:12">
       <c r="A131" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B131" t="s">
         <v>585</v>
@@ -7956,7 +7947,7 @@
         <v>695</v>
       </c>
       <c r="J131" s="5" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="K131">
         <v>41.831244439999999</v>
@@ -7967,7 +7958,7 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B132" t="s">
         <v>586</v>
@@ -7994,7 +7985,7 @@
         <v>696</v>
       </c>
       <c r="J132" s="5" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="K132">
         <v>41.037952779999998</v>
@@ -8005,7 +7996,7 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B133" t="s">
         <v>587</v>
@@ -8032,7 +8023,7 @@
         <v>697</v>
       </c>
       <c r="J133" s="5" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="K133">
         <v>41.032444439999999</v>
@@ -8043,7 +8034,7 @@
     </row>
     <row r="134" spans="1:12">
       <c r="A134" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B134" t="s">
         <v>588</v>
@@ -8070,7 +8061,7 @@
         <v>698</v>
       </c>
       <c r="J134" s="5" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="K134">
         <v>40.893113890000002</v>
@@ -8081,7 +8072,7 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B135" t="s">
         <v>589</v>
@@ -8108,7 +8099,7 @@
         <v>699</v>
       </c>
       <c r="J135" s="5" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="K135">
         <v>41.01569722</v>
@@ -8119,7 +8110,7 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B136" t="s">
         <v>590</v>
@@ -8146,7 +8137,7 @@
         <v>700</v>
       </c>
       <c r="J136" s="5" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="K136">
         <v>39.94777732</v>
@@ -8157,7 +8148,7 @@
     </row>
     <row r="137" spans="1:12">
       <c r="A137" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B137" t="s">
         <v>591</v>
@@ -8184,7 +8175,7 @@
         <v>701</v>
       </c>
       <c r="J137" s="5" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="K137">
         <v>39.985005569999998</v>
@@ -8195,7 +8186,7 @@
     </row>
     <row r="138" spans="1:12">
       <c r="A138" t="s">
-        <v>723</v>
+        <v>779</v>
       </c>
       <c r="B138" t="s">
         <v>592</v>
@@ -8222,7 +8213,7 @@
         <v>702</v>
       </c>
       <c r="J138" s="5" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="K138">
         <v>40.120006940000003</v>
@@ -8233,7 +8224,7 @@
     </row>
     <row r="139" spans="1:12">
       <c r="A139" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B139" t="s">
         <v>593</v>
@@ -8260,7 +8251,7 @@
         <v>703</v>
       </c>
       <c r="J139" s="5" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="K139">
         <v>39.769849219999998</v>
@@ -8271,7 +8262,7 @@
     </row>
     <row r="140" spans="1:12">
       <c r="A140" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B140" t="s">
         <v>594</v>
@@ -8298,7 +8289,7 @@
         <v>704</v>
       </c>
       <c r="J140" s="5" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="K140">
         <v>39.899249439999998</v>
@@ -8309,7 +8300,7 @@
     </row>
     <row r="141" spans="1:12">
       <c r="A141" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B141" t="s">
         <v>595</v>
@@ -8336,7 +8327,7 @@
         <v>705</v>
       </c>
       <c r="J141" s="5" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="K141">
         <v>39.139068760000001</v>
@@ -8347,7 +8338,7 @@
     </row>
     <row r="142" spans="1:12">
       <c r="A142" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B142" t="s">
         <v>596</v>
@@ -8374,7 +8365,7 @@
         <v>706</v>
       </c>
       <c r="J142" s="5" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="K142">
         <v>39.031109000000001</v>
@@ -8385,7 +8376,7 @@
     </row>
     <row r="143" spans="1:12">
       <c r="A143" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B143" t="s">
         <v>597</v>
@@ -8412,7 +8403,7 @@
         <v>707</v>
       </c>
       <c r="J143" s="5" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="K143">
         <v>39.681924049999999</v>
@@ -8423,7 +8414,7 @@
     </row>
     <row r="144" spans="1:12">
       <c r="A144" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B144" t="s">
         <v>598</v>
@@ -8450,7 +8441,7 @@
         <v>708</v>
       </c>
       <c r="J144" s="5" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="K144">
         <v>39.062654530000003</v>
@@ -8461,7 +8452,7 @@
     </row>
     <row r="145" spans="1:12">
       <c r="A145" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B145" t="s">
         <v>599</v>
@@ -8488,7 +8479,7 @@
         <v>709</v>
       </c>
       <c r="J145" s="5" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="K145">
         <v>39.238330240000003</v>
@@ -8499,7 +8490,7 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B146" t="s">
         <v>600</v>
@@ -8526,7 +8517,7 @@
         <v>710</v>
       </c>
       <c r="J146" s="5" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="K146">
         <v>39.099380029999999</v>
@@ -8537,7 +8528,7 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B147" t="s">
         <v>601</v>
@@ -8564,7 +8555,7 @@
         <v>711</v>
       </c>
       <c r="J147" s="5" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="K147">
         <v>39.116327339999998</v>
@@ -8575,7 +8566,7 @@
     </row>
     <row r="148" spans="1:12">
       <c r="A148" t="s">
-        <v>726</v>
+        <v>781</v>
       </c>
       <c r="B148" t="s">
         <v>602</v>
@@ -8602,7 +8593,7 @@
         <v>712</v>
       </c>
       <c r="J148" s="5" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="K148">
         <v>40.309908329999999</v>
@@ -8613,7 +8604,7 @@
     </row>
     <row r="149" spans="1:12">
       <c r="A149" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B149" t="s">
         <v>603</v>
@@ -8640,7 +8631,7 @@
         <v>713</v>
       </c>
       <c r="J149" s="5" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="K149">
         <v>38.56700524</v>
@@ -8651,7 +8642,7 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B150" t="s">
         <v>604</v>
@@ -8678,7 +8669,7 @@
         <v>714</v>
       </c>
       <c r="J150" s="5" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="K150">
         <v>38.710690339999999</v>
@@ -8689,7 +8680,7 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B151" t="s">
         <v>605</v>
@@ -8716,7 +8707,7 @@
         <v>715</v>
       </c>
       <c r="J151" s="5" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="K151">
         <v>38.018968280000003</v>
@@ -8727,7 +8718,7 @@
     </row>
     <row r="152" spans="1:12">
       <c r="A152" t="s">
-        <v>726</v>
+        <v>781</v>
       </c>
       <c r="B152" t="s">
         <v>606</v>
@@ -8754,7 +8745,7 @@
         <v>716</v>
       </c>
       <c r="J152" s="5" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="K152">
         <v>37.402369440000001</v>
@@ -8765,7 +8756,7 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" t="s">
-        <v>726</v>
+        <v>781</v>
       </c>
       <c r="B153" t="s">
         <v>607</v>
@@ -8792,7 +8783,7 @@
         <v>717</v>
       </c>
       <c r="J153" s="5" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="K153">
         <v>37.682652779999998</v>
@@ -8803,7 +8794,7 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" t="s">
-        <v>726</v>
+        <v>781</v>
       </c>
       <c r="B154" t="s">
         <v>608</v>
@@ -8830,7 +8821,7 @@
         <v>718</v>
       </c>
       <c r="J154" s="5" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="K154">
         <v>37.750466670000002</v>

</xml_diff>

<commit_message>
Fixed the X axis with xlim
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_annual.xlsx
+++ b/code/paleo_flow/data/sites_annual.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="862">
   <si>
     <t xml:space="preserve">orig_order</t>
   </si>
@@ -2576,6 +2576,36 @@
   </si>
   <si>
     <t xml:space="preserve">yellowstone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ping River at Nawarat Bridge, Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hung T.T. Nguyen;  Stefano Galelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyen, H. T. T., &amp; Galelli, S. (2018). A Linear Dynamical Systems Approach to Streamflow Reconstruction Reveals History of Regime Shifts in Northern Thailand. Water Resources Research, 54(3), 2057–2077. https://doi.org/10.1002/2017WR022114 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ntthung/ldsr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gauge P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royal Irrigation Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.hydro-1.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Year (April-March)</t>
   </si>
 </sst>
 </file>
@@ -2838,10 +2868,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W159"/>
+  <dimension ref="A1:W160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K78" activeCellId="0" sqref="K78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A160" activeCellId="0" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11075,6 +11105,47 @@
       </c>
       <c r="M159" s="0" t="n">
         <v>-110.793667</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="C160" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="F160" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="H160" s="0" t="s">
+        <v>857</v>
+      </c>
+      <c r="I160" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="J160" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="K160" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="L160" s="0" t="n">
+        <v>18.78766</v>
+      </c>
+      <c r="M160" s="0" t="n">
+        <v>99.00443</v>
+      </c>
+      <c r="N160" s="0" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>
@@ -11162,6 +11233,7 @@
     <hyperlink ref="G154" r:id="rId81" display="https://www.treeflow.info/content/santa-ana-river"/>
     <hyperlink ref="J158" r:id="rId82" display="https://hydrowebportal.niwa.co.nz/Data/DataSet/Summary/Location/65104/DataSet/QR/Master/Interval/Latest"/>
     <hyperlink ref="J159" r:id="rId83" display="https://waterdata.usgs.gov/nwis/inventory/?site_no=06191500&amp;agency_cd=USGS"/>
+    <hyperlink ref="J160" r:id="rId84" display="https://www.hydro-1.net"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fixed the header, ready to upload
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_annual.xlsx
+++ b/code/paleo_flow/data/sites_annual.xlsx
@@ -2870,8 +2870,8 @@
   </sheetPr>
   <dimension ref="A1:W160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A160" activeCellId="0" sqref="A160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4040,10 +4040,10 @@
         <v>0.8</v>
       </c>
       <c r="R19" s="0" t="n">
-        <v>18.41</v>
+        <v>1.841</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>19.45</v>
+        <v>1.945</v>
       </c>
       <c r="U19" s="0" t="s">
         <v>129</v>
@@ -4093,10 +4093,10 @@
         <v>0.55</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>27.84</v>
+        <v>2.784</v>
       </c>
       <c r="S20" s="0" t="n">
-        <v>29.29</v>
+        <v>2.929</v>
       </c>
       <c r="U20" s="0" t="s">
         <v>129</v>

</xml_diff>